<commit_message>
Updated Voice Line V
</commit_message>
<xml_diff>
--- a/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_VoiceLine.xlsx
+++ b/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_VoiceLine.xlsx
@@ -1086,9 +1086,6 @@
     <t>Remove Configuration</t>
   </si>
   <si>
-    <t>Si_E17</t>
-  </si>
-  <si>
     <t>VLV8720</t>
   </si>
   <si>
@@ -1144,6 +1141,9 @@
   </si>
   <si>
     <t>vlvedit8720@test.com</t>
+  </si>
+  <si>
+    <t>Si_E19</t>
   </si>
 </sst>
 </file>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="DZ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="EE5" sqref="EE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2539,34 +2539,34 @@
     </row>
     <row r="2" spans="1:261" ht="27" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>204</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>79</v>
@@ -2587,7 +2587,7 @@
         <v>22</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>5</v>
@@ -2596,22 +2596,22 @@
         <v>6</v>
       </c>
       <c r="T2" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="U2" s="7" t="s">
-        <v>363</v>
-      </c>
       <c r="V2" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>363</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>25</v>
@@ -2644,10 +2644,10 @@
         <v>44</v>
       </c>
       <c r="AJ2" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="AK2" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="AK2" s="7" t="s">
-        <v>366</v>
       </c>
       <c r="AL2" s="7" t="s">
         <v>26</v>
@@ -2656,19 +2656,19 @@
         <v>49</v>
       </c>
       <c r="AN2" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AO2" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AP2" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AR2" s="7" t="s">
         <v>369</v>
-      </c>
-      <c r="AR2" s="7" t="s">
-        <v>370</v>
       </c>
       <c r="AS2" s="7" t="s">
         <v>77</v>
@@ -2677,7 +2677,7 @@
         <v>62</v>
       </c>
       <c r="AU2" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AV2" s="7" t="s">
         <v>78</v>
@@ -2692,16 +2692,16 @@
         <v>75</v>
       </c>
       <c r="AZ2" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="BA2" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="BA2" s="7" t="s">
-        <v>373</v>
-      </c>
       <c r="BB2" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="BC2" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="BC2" s="7" t="s">
-        <v>363</v>
       </c>
       <c r="BD2" s="7" t="s">
         <v>65</v>
@@ -2740,7 +2740,7 @@
         <v>88</v>
       </c>
       <c r="BP2" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="BQ2" s="7" t="s">
         <v>96</v>
@@ -2941,7 +2941,7 @@
         <v>88</v>
       </c>
       <c r="EE2" s="13" t="s">
-        <v>355</v>
+        <v>374</v>
       </c>
       <c r="EF2" s="13" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Updated VLV test data sheet
</commit_message>
<xml_diff>
--- a/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_VoiceLine.xlsx
+++ b/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_VoiceLine.xlsx
@@ -1143,7 +1143,7 @@
     <t>vlvedit8720@test.com</t>
   </si>
   <si>
-    <t>Si_E19</t>
+    <t>Si_E34</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1570,7 @@
   <dimension ref="A1:JA2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="DZ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EE5" sqref="EE5"/>
+      <selection activeCell="ED7" sqref="ED7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>